<commit_message>
update workbook dec 8
</commit_message>
<xml_diff>
--- a/Learning Time Frame.xlsx
+++ b/Learning Time Frame.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="84">
   <si>
     <t>Topic ID</t>
   </si>
@@ -87,9 +87,6 @@
   </si>
   <si>
     <t>Version History</t>
-  </si>
-  <si>
-    <t>In Progress</t>
   </si>
   <si>
     <t>https://docs.google.com/document/d/13SlpZbMJ52VxuuaGhp9Z7lY60it2GHCgS44sJsr6iWQ/edit?usp=sharing</t>
@@ -952,12 +949,14 @@
       <c r="E6" s="12">
         <v>45995.0</v>
       </c>
-      <c r="F6" s="13"/>
+      <c r="F6" s="12">
+        <v>45995.0</v>
+      </c>
       <c r="G6" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="15" t="s">
         <v>24</v>
-      </c>
-      <c r="H6" s="15" t="s">
-        <v>25</v>
       </c>
       <c r="I6" s="9" t="s">
         <v>13</v>
@@ -7985,19 +7984,19 @@
   <sheetData>
     <row r="1" ht="22.5" customHeight="1">
       <c r="A1" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="C1" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="D1" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="E1" s="20" t="s">
         <v>29</v>
-      </c>
-      <c r="E1" s="20" t="s">
-        <v>30</v>
       </c>
       <c r="F1" s="20" t="s">
         <v>4</v>
@@ -8006,10 +8005,10 @@
         <v>5</v>
       </c>
       <c r="H1" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="20" t="s">
         <v>31</v>
-      </c>
-      <c r="I1" s="20" t="s">
-        <v>32</v>
       </c>
       <c r="J1" s="22"/>
       <c r="K1" s="22"/>
@@ -8024,7 +8023,7 @@
         <v>1001.0</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" s="25" t="s">
         <v>9</v>
@@ -8045,7 +8044,7 @@
         <v>11</v>
       </c>
       <c r="I2" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J2" s="27"/>
       <c r="K2" s="27"/>
@@ -8060,7 +8059,7 @@
         <v>1002.0</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" s="25" t="s">
         <v>9</v>
@@ -8081,7 +8080,7 @@
         <v>11</v>
       </c>
       <c r="I3" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J3" s="27"/>
       <c r="K3" s="27"/>
@@ -8096,7 +8095,7 @@
         <v>1003.0</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C4" s="25" t="s">
         <v>9</v>
@@ -8117,7 +8116,7 @@
         <v>11</v>
       </c>
       <c r="I4" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J4" s="27"/>
       <c r="K4" s="27"/>
@@ -8132,7 +8131,7 @@
         <v>1004.0</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C5" s="25" t="s">
         <v>9</v>
@@ -8153,7 +8152,7 @@
         <v>11</v>
       </c>
       <c r="I5" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J5" s="27"/>
       <c r="K5" s="27"/>
@@ -8168,7 +8167,7 @@
         <v>2001.0</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>14</v>
@@ -8189,7 +8188,7 @@
         <v>11</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" ht="22.5" customHeight="1">
@@ -8197,7 +8196,7 @@
         <v>2002.0</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>14</v>
@@ -8224,7 +8223,7 @@
         <v>2003.0</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>14</v>
@@ -8245,7 +8244,7 @@
         <v>11</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" ht="22.5" customHeight="1">
@@ -8253,7 +8252,7 @@
         <v>3001.0</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>16</v>
@@ -8274,7 +8273,7 @@
         <v>11</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" ht="22.5" customHeight="1">
@@ -8282,7 +8281,7 @@
         <v>3002.0</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>16</v>
@@ -8303,7 +8302,7 @@
         <v>11</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" ht="22.5" customHeight="1">
@@ -8311,7 +8310,7 @@
         <v>3003.0</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>16</v>
@@ -8332,7 +8331,7 @@
         <v>11</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" ht="22.5" customHeight="1">
@@ -8340,7 +8339,7 @@
         <v>3004.0</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>16</v>
@@ -8361,7 +8360,7 @@
         <v>11</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" ht="22.5" customHeight="1">
@@ -8369,7 +8368,7 @@
         <v>3005.0</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>16</v>
@@ -8390,7 +8389,7 @@
         <v>11</v>
       </c>
       <c r="I13" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" ht="22.5" customHeight="1">
@@ -8398,7 +8397,7 @@
         <v>3006.0</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>16</v>
@@ -8419,7 +8418,7 @@
         <v>11</v>
       </c>
       <c r="I14" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" ht="22.5" customHeight="1">
@@ -8427,7 +8426,7 @@
         <v>3007.0</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>16</v>
@@ -8448,7 +8447,7 @@
         <v>11</v>
       </c>
       <c r="I15" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" ht="22.5" customHeight="1">
@@ -8456,7 +8455,7 @@
         <v>3008.0</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>16</v>
@@ -8477,7 +8476,7 @@
         <v>11</v>
       </c>
       <c r="I16" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" ht="22.5" customHeight="1">
@@ -8485,7 +8484,7 @@
         <v>3009.0</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>16</v>
@@ -8506,7 +8505,7 @@
         <v>11</v>
       </c>
       <c r="I17" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" ht="22.5" customHeight="1">
@@ -8514,7 +8513,7 @@
         <v>4001.0</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>19</v>
@@ -8535,7 +8534,7 @@
         <v>11</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" ht="22.5" customHeight="1">
@@ -8543,7 +8542,7 @@
         <v>4002.0</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>19</v>
@@ -8564,7 +8563,7 @@
         <v>11</v>
       </c>
       <c r="I19" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" ht="22.5" customHeight="1">
@@ -8572,7 +8571,7 @@
         <v>4003.0</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>19</v>
@@ -8593,7 +8592,7 @@
         <v>11</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" ht="22.5" customHeight="1">
@@ -8601,7 +8600,7 @@
         <v>4004.0</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>19</v>
@@ -8622,7 +8621,7 @@
         <v>11</v>
       </c>
       <c r="I21" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" ht="22.5" customHeight="1">
@@ -8630,7 +8629,7 @@
         <v>4005.0</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>19</v>
@@ -8651,7 +8650,7 @@
         <v>11</v>
       </c>
       <c r="I22" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" ht="22.5" customHeight="1">
@@ -8659,7 +8658,7 @@
         <v>4006.0</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>19</v>
@@ -8680,7 +8679,7 @@
         <v>11</v>
       </c>
       <c r="I23" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" ht="22.5" customHeight="1">
@@ -8688,7 +8687,7 @@
         <v>4007.0</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>19</v>
@@ -8709,7 +8708,7 @@
         <v>11</v>
       </c>
       <c r="I24" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" ht="22.5" customHeight="1">
@@ -8717,7 +8716,7 @@
         <v>4008.0</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>19</v>
@@ -8738,7 +8737,7 @@
         <v>11</v>
       </c>
       <c r="I25" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" ht="22.5" customHeight="1">
@@ -8746,7 +8745,7 @@
         <v>4009.0</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>19</v>
@@ -8767,7 +8766,7 @@
         <v>11</v>
       </c>
       <c r="I26" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" ht="22.5" customHeight="1">
@@ -8775,7 +8774,7 @@
         <v>4010.0</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>19</v>
@@ -8796,7 +8795,7 @@
         <v>11</v>
       </c>
       <c r="I27" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" ht="22.5" customHeight="1">
@@ -8804,7 +8803,7 @@
         <v>4011.0</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>19</v>
@@ -8825,7 +8824,7 @@
         <v>11</v>
       </c>
       <c r="I28" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" ht="22.5" customHeight="1">
@@ -8833,7 +8832,7 @@
         <v>4012.0</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>19</v>
@@ -8854,7 +8853,7 @@
         <v>11</v>
       </c>
       <c r="I29" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" ht="22.5" customHeight="1">
@@ -8862,7 +8861,7 @@
         <v>4013.0</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>19</v>
@@ -8883,7 +8882,7 @@
         <v>11</v>
       </c>
       <c r="I30" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" ht="22.5" customHeight="1">
@@ -8891,7 +8890,7 @@
         <v>5001.0</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C31" s="14" t="s">
         <v>22</v>
@@ -8912,7 +8911,7 @@
         <v>11</v>
       </c>
       <c r="I31" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" ht="22.5" customHeight="1">
@@ -8920,7 +8919,7 @@
         <v>5002.0</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C32" s="14" t="s">
         <v>22</v>
@@ -8941,7 +8940,7 @@
         <v>11</v>
       </c>
       <c r="I32" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33" ht="22.5" customHeight="1">
@@ -8949,7 +8948,7 @@
         <v>5003.0</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C33" s="14" t="s">
         <v>22</v>
@@ -8970,7 +8969,7 @@
         <v>11</v>
       </c>
       <c r="I33" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" ht="22.5" customHeight="1">
@@ -8978,7 +8977,7 @@
         <v>5004.0</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C34" s="14" t="s">
         <v>22</v>
@@ -8999,7 +8998,7 @@
         <v>11</v>
       </c>
       <c r="I34" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35" ht="22.5" customHeight="1">
@@ -9007,7 +9006,7 @@
         <v>5005.0</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C35" s="14" t="s">
         <v>22</v>
@@ -9028,7 +9027,7 @@
         <v>11</v>
       </c>
       <c r="I35" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="36" ht="22.5" customHeight="1">
@@ -9036,7 +9035,7 @@
         <v>5006.0</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C36" s="14" t="s">
         <v>22</v>
@@ -9057,7 +9056,7 @@
         <v>11</v>
       </c>
       <c r="I36" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="37" ht="22.5" customHeight="1">
@@ -9065,7 +9064,7 @@
         <v>5007.0</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C37" s="14" t="s">
         <v>22</v>
@@ -9086,7 +9085,7 @@
         <v>11</v>
       </c>
       <c r="I37" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38" ht="22.5" customHeight="1">
@@ -9094,7 +9093,7 @@
         <v>5008.0</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C38" s="14" t="s">
         <v>22</v>
@@ -9115,7 +9114,7 @@
         <v>11</v>
       </c>
       <c r="I38" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="39" ht="22.5" customHeight="1">
@@ -9123,7 +9122,7 @@
         <v>5009.0</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C39" s="14" t="s">
         <v>22</v>
@@ -9137,12 +9136,14 @@
       <c r="F39" s="12">
         <v>45993.0</v>
       </c>
-      <c r="G39" s="12"/>
+      <c r="G39" s="12">
+        <v>45995.0</v>
+      </c>
       <c r="H39" s="14" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="I39" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="40" ht="22.5" customHeight="1">
@@ -9150,7 +9151,7 @@
         <v>5010.0</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C40" s="14" t="s">
         <v>22</v>
@@ -9171,7 +9172,7 @@
         <v>11</v>
       </c>
       <c r="I40" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="41" ht="22.5" customHeight="1">
@@ -9179,7 +9180,7 @@
         <v>5011.0</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C41" s="14" t="s">
         <v>22</v>
@@ -9200,7 +9201,7 @@
         <v>11</v>
       </c>
       <c r="I41" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="42" ht="22.5" customHeight="1">
@@ -15959,42 +15960,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="28" t="s">
         <v>75</v>
-      </c>
-      <c r="B1" s="28" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="28" t="s">
         <v>77</v>
-      </c>
-      <c r="B2" s="28" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="28" t="s">
         <v>79</v>
-      </c>
-      <c r="B3" s="28" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="28" t="s">
         <v>81</v>
-      </c>
-      <c r="B4" s="28" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" s="28" t="s">
         <v>83</v>
-      </c>
-      <c r="B5" s="28" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Sheet Jan 5
</commit_message>
<xml_diff>
--- a/Learning Time Frame.xlsx
+++ b/Learning Time Frame.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="109">
   <si>
     <t>Topic ID</t>
   </si>
@@ -95,9 +95,6 @@
     <t>LLM &amp; OLLAMA</t>
   </si>
   <si>
-    <t>Paused</t>
-  </si>
-  <si>
     <t>https://docs.google.com/document/d/14-Q2IgtfvNJwmBoZqeULPpvTZovfszjBHF2Vv3Vc3iU/edit?usp=sharing</t>
   </si>
   <si>
@@ -105,9 +102,6 @@
   </si>
   <si>
     <t>ETL</t>
-  </si>
-  <si>
-    <t>In Progress</t>
   </si>
   <si>
     <t>https://docs.google.com/document/d/1eHKCZNTIX_QTt0o6KbOMXg-zNPqDYupqx0NvrNOm9tI/edit?usp=sharing</t>
@@ -306,9 +300,6 @@
   </si>
   <si>
     <t>Glue Workflows &amp; Triggers</t>
-  </si>
-  <si>
-    <t>Not Started</t>
   </si>
   <si>
     <t>Glue Studio &amp; Visual ETL</t>
@@ -1067,12 +1058,14 @@
       <c r="E7" s="12">
         <v>46014.0</v>
       </c>
-      <c r="F7" s="13"/>
+      <c r="F7" s="12">
+        <v>46007.0</v>
+      </c>
       <c r="G7" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="15" t="s">
         <v>26</v>
-      </c>
-      <c r="H7" s="15" t="s">
-        <v>27</v>
       </c>
       <c r="I7" s="9" t="s">
         <v>13</v>
@@ -1083,23 +1076,25 @@
         <v>7000.0</v>
       </c>
       <c r="B8" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>28</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>29</v>
       </c>
       <c r="D8" s="12">
         <v>46008.0</v>
       </c>
       <c r="E8" s="12">
-        <v>46026.0</v>
-      </c>
-      <c r="F8" s="13"/>
+        <v>46028.0</v>
+      </c>
+      <c r="F8" s="12">
+        <v>46027.0</v>
+      </c>
       <c r="G8" s="14" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I8" s="9" t="s">
         <v>13</v>
@@ -8111,19 +8106,19 @@
   <sheetData>
     <row r="1" ht="22.5" customHeight="1">
       <c r="A1" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="D1" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="E1" s="18" t="s">
         <v>34</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>36</v>
       </c>
       <c r="F1" s="18" t="s">
         <v>4</v>
@@ -8132,10 +8127,10 @@
         <v>5</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I1" s="18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J1" s="20"/>
       <c r="K1" s="20"/>
@@ -8150,7 +8145,7 @@
         <v>1001.0</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C2" s="23" t="s">
         <v>9</v>
@@ -8171,7 +8166,7 @@
         <v>11</v>
       </c>
       <c r="I2" s="22" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J2" s="25"/>
       <c r="K2" s="25"/>
@@ -8186,7 +8181,7 @@
         <v>1002.0</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C3" s="23" t="s">
         <v>9</v>
@@ -8207,7 +8202,7 @@
         <v>11</v>
       </c>
       <c r="I3" s="22" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J3" s="25"/>
       <c r="K3" s="25"/>
@@ -8222,7 +8217,7 @@
         <v>1003.0</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C4" s="23" t="s">
         <v>9</v>
@@ -8243,7 +8238,7 @@
         <v>11</v>
       </c>
       <c r="I4" s="22" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J4" s="25"/>
       <c r="K4" s="25"/>
@@ -8258,7 +8253,7 @@
         <v>1004.0</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C5" s="23" t="s">
         <v>9</v>
@@ -8279,7 +8274,7 @@
         <v>11</v>
       </c>
       <c r="I5" s="22" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J5" s="25"/>
       <c r="K5" s="25"/>
@@ -8294,7 +8289,7 @@
         <v>2001.0</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>14</v>
@@ -8315,7 +8310,7 @@
         <v>11</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" ht="22.5" customHeight="1">
@@ -8323,7 +8318,7 @@
         <v>2002.0</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>14</v>
@@ -8350,7 +8345,7 @@
         <v>2003.0</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>14</v>
@@ -8371,7 +8366,7 @@
         <v>11</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" ht="22.5" customHeight="1">
@@ -8379,7 +8374,7 @@
         <v>3001.0</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>16</v>
@@ -8400,7 +8395,7 @@
         <v>11</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" ht="22.5" customHeight="1">
@@ -8408,7 +8403,7 @@
         <v>3002.0</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>16</v>
@@ -8429,7 +8424,7 @@
         <v>11</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" ht="22.5" customHeight="1">
@@ -8437,7 +8432,7 @@
         <v>3003.0</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>16</v>
@@ -8458,7 +8453,7 @@
         <v>11</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" ht="22.5" customHeight="1">
@@ -8466,7 +8461,7 @@
         <v>3004.0</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>16</v>
@@ -8487,7 +8482,7 @@
         <v>11</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" ht="22.5" customHeight="1">
@@ -8495,7 +8490,7 @@
         <v>3005.0</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>16</v>
@@ -8516,7 +8511,7 @@
         <v>11</v>
       </c>
       <c r="I13" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" ht="22.5" customHeight="1">
@@ -8524,7 +8519,7 @@
         <v>3006.0</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>16</v>
@@ -8545,7 +8540,7 @@
         <v>11</v>
       </c>
       <c r="I14" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" ht="22.5" customHeight="1">
@@ -8553,7 +8548,7 @@
         <v>3007.0</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>16</v>
@@ -8574,7 +8569,7 @@
         <v>11</v>
       </c>
       <c r="I15" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" ht="22.5" customHeight="1">
@@ -8582,7 +8577,7 @@
         <v>3008.0</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>16</v>
@@ -8603,7 +8598,7 @@
         <v>11</v>
       </c>
       <c r="I16" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" ht="22.5" customHeight="1">
@@ -8611,7 +8606,7 @@
         <v>3009.0</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>16</v>
@@ -8632,7 +8627,7 @@
         <v>11</v>
       </c>
       <c r="I17" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" ht="22.5" customHeight="1">
@@ -8640,7 +8635,7 @@
         <v>4001.0</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>19</v>
@@ -8661,7 +8656,7 @@
         <v>11</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" ht="22.5" customHeight="1">
@@ -8669,7 +8664,7 @@
         <v>4002.0</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>19</v>
@@ -8690,7 +8685,7 @@
         <v>11</v>
       </c>
       <c r="I19" s="11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" ht="22.5" customHeight="1">
@@ -8698,7 +8693,7 @@
         <v>4003.0</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>19</v>
@@ -8719,7 +8714,7 @@
         <v>11</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" ht="22.5" customHeight="1">
@@ -8727,7 +8722,7 @@
         <v>4004.0</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>19</v>
@@ -8748,7 +8743,7 @@
         <v>11</v>
       </c>
       <c r="I21" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" ht="22.5" customHeight="1">
@@ -8756,7 +8751,7 @@
         <v>4005.0</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>19</v>
@@ -8777,7 +8772,7 @@
         <v>11</v>
       </c>
       <c r="I22" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" ht="22.5" customHeight="1">
@@ -8785,7 +8780,7 @@
         <v>4006.0</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>19</v>
@@ -8806,7 +8801,7 @@
         <v>11</v>
       </c>
       <c r="I23" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" ht="22.5" customHeight="1">
@@ -8814,7 +8809,7 @@
         <v>4007.0</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>19</v>
@@ -8835,7 +8830,7 @@
         <v>11</v>
       </c>
       <c r="I24" s="11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" ht="22.5" customHeight="1">
@@ -8843,7 +8838,7 @@
         <v>4008.0</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>19</v>
@@ -8864,7 +8859,7 @@
         <v>11</v>
       </c>
       <c r="I25" s="11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" ht="22.5" customHeight="1">
@@ -8872,7 +8867,7 @@
         <v>4009.0</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>19</v>
@@ -8893,7 +8888,7 @@
         <v>11</v>
       </c>
       <c r="I26" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" ht="22.5" customHeight="1">
@@ -8901,7 +8896,7 @@
         <v>4010.0</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>19</v>
@@ -8922,7 +8917,7 @@
         <v>11</v>
       </c>
       <c r="I27" s="11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" ht="22.5" customHeight="1">
@@ -8930,7 +8925,7 @@
         <v>4011.0</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>19</v>
@@ -8951,7 +8946,7 @@
         <v>11</v>
       </c>
       <c r="I28" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" ht="22.5" customHeight="1">
@@ -8959,7 +8954,7 @@
         <v>4012.0</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>19</v>
@@ -8980,7 +8975,7 @@
         <v>11</v>
       </c>
       <c r="I29" s="11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" ht="22.5" customHeight="1">
@@ -8988,7 +8983,7 @@
         <v>4013.0</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>19</v>
@@ -9009,7 +9004,7 @@
         <v>11</v>
       </c>
       <c r="I30" s="11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" ht="22.5" customHeight="1">
@@ -9017,7 +9012,7 @@
         <v>5001.0</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C31" s="14" t="s">
         <v>22</v>
@@ -9038,7 +9033,7 @@
         <v>11</v>
       </c>
       <c r="I31" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" ht="22.5" customHeight="1">
@@ -9046,7 +9041,7 @@
         <v>5002.0</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C32" s="14" t="s">
         <v>22</v>
@@ -9067,7 +9062,7 @@
         <v>11</v>
       </c>
       <c r="I32" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" ht="22.5" customHeight="1">
@@ -9075,7 +9070,7 @@
         <v>5003.0</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C33" s="14" t="s">
         <v>22</v>
@@ -9096,7 +9091,7 @@
         <v>11</v>
       </c>
       <c r="I33" s="11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" ht="22.5" customHeight="1">
@@ -9104,7 +9099,7 @@
         <v>5004.0</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C34" s="14" t="s">
         <v>22</v>
@@ -9125,7 +9120,7 @@
         <v>11</v>
       </c>
       <c r="I34" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" ht="22.5" customHeight="1">
@@ -9133,7 +9128,7 @@
         <v>5005.0</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C35" s="14" t="s">
         <v>22</v>
@@ -9154,7 +9149,7 @@
         <v>11</v>
       </c>
       <c r="I35" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="36" ht="22.5" customHeight="1">
@@ -9162,7 +9157,7 @@
         <v>5006.0</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C36" s="14" t="s">
         <v>22</v>
@@ -9183,7 +9178,7 @@
         <v>11</v>
       </c>
       <c r="I36" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="37" ht="22.5" customHeight="1">
@@ -9191,7 +9186,7 @@
         <v>5007.0</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C37" s="14" t="s">
         <v>22</v>
@@ -9212,7 +9207,7 @@
         <v>11</v>
       </c>
       <c r="I37" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="38" ht="22.5" customHeight="1">
@@ -9220,7 +9215,7 @@
         <v>5008.0</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C38" s="14" t="s">
         <v>22</v>
@@ -9241,7 +9236,7 @@
         <v>11</v>
       </c>
       <c r="I38" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="39" ht="22.5" customHeight="1">
@@ -9249,7 +9244,7 @@
         <v>5009.0</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C39" s="14" t="s">
         <v>22</v>
@@ -9270,7 +9265,7 @@
         <v>11</v>
       </c>
       <c r="I39" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="40" ht="22.5" customHeight="1">
@@ -9278,7 +9273,7 @@
         <v>5010.0</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C40" s="14" t="s">
         <v>22</v>
@@ -9299,7 +9294,7 @@
         <v>11</v>
       </c>
       <c r="I40" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="41" ht="22.5" customHeight="1">
@@ -9307,7 +9302,7 @@
         <v>5011.0</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C41" s="14" t="s">
         <v>22</v>
@@ -9328,7 +9323,7 @@
         <v>11</v>
       </c>
       <c r="I41" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="42" ht="22.5" customHeight="1">
@@ -9336,7 +9331,7 @@
         <v>5012.0</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C42" s="14" t="s">
         <v>22</v>
@@ -9357,7 +9352,7 @@
         <v>11</v>
       </c>
       <c r="I42" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="43" ht="22.5" customHeight="1">
@@ -9365,7 +9360,7 @@
         <v>5013.0</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C43" s="14" t="s">
         <v>22</v>
@@ -9386,7 +9381,7 @@
         <v>11</v>
       </c>
       <c r="I43" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="44" ht="22.5" customHeight="1">
@@ -9394,7 +9389,7 @@
         <v>5014.0</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C44" s="14" t="s">
         <v>22</v>
@@ -9415,7 +9410,7 @@
         <v>11</v>
       </c>
       <c r="I44" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="45" ht="22.5" customHeight="1">
@@ -9423,7 +9418,7 @@
         <v>6001.0</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C45" s="14" t="s">
         <v>25</v>
@@ -9444,7 +9439,7 @@
         <v>11</v>
       </c>
       <c r="I45" s="11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" ht="22.5" customHeight="1">
@@ -9452,7 +9447,7 @@
         <v>6002.0</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C46" s="14" t="s">
         <v>25</v>
@@ -9473,7 +9468,7 @@
         <v>11</v>
       </c>
       <c r="I46" s="11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="47" ht="22.5" customHeight="1">
@@ -9481,7 +9476,7 @@
         <v>6003.0</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C47" s="14" t="s">
         <v>25</v>
@@ -9502,7 +9497,7 @@
         <v>11</v>
       </c>
       <c r="I47" s="11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="48" ht="22.5" customHeight="1">
@@ -9510,7 +9505,7 @@
         <v>6004.0</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C48" s="14" t="s">
         <v>25</v>
@@ -9531,7 +9526,7 @@
         <v>11</v>
       </c>
       <c r="I48" s="11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="49" ht="22.5" customHeight="1">
@@ -9539,7 +9534,7 @@
         <v>6005.0</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C49" s="14" t="s">
         <v>25</v>
@@ -9547,25 +9542,31 @@
       <c r="D49" s="12">
         <v>46013.0</v>
       </c>
-      <c r="E49" s="12"/>
+      <c r="E49" s="12">
+        <v>46007.0</v>
+      </c>
       <c r="F49" s="12">
         <v>46014.0</v>
       </c>
-      <c r="G49" s="12"/>
+      <c r="G49" s="12">
+        <v>46007.0</v>
+      </c>
       <c r="H49" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="I49" s="11"/>
+        <v>11</v>
+      </c>
+      <c r="I49" s="11" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="50" ht="22.5" customHeight="1">
       <c r="A50" s="10">
         <v>7001.0</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C50" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D50" s="12">
         <v>46008.0</v>
@@ -9583,7 +9584,7 @@
         <v>11</v>
       </c>
       <c r="I50" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="51" ht="22.5" customHeight="1">
@@ -9591,10 +9592,10 @@
         <v>7002.0</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C51" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D51" s="12">
         <v>46009.0</v>
@@ -9612,7 +9613,7 @@
         <v>11</v>
       </c>
       <c r="I51" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="52" ht="22.5" customHeight="1">
@@ -9620,10 +9621,10 @@
         <v>7003.0</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C52" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D52" s="12">
         <v>46013.0</v>
@@ -9641,7 +9642,7 @@
         <v>11</v>
       </c>
       <c r="I52" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="53" ht="22.5" customHeight="1">
@@ -9649,10 +9650,10 @@
         <v>7004.0</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C53" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D53" s="12">
         <v>46014.0</v>
@@ -9670,7 +9671,7 @@
         <v>11</v>
       </c>
       <c r="I53" s="11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="54" ht="22.5" customHeight="1">
@@ -9678,10 +9679,10 @@
         <v>7005.0</v>
       </c>
       <c r="B54" s="11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C54" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D54" s="12">
         <v>46020.0</v>
@@ -9699,7 +9700,7 @@
         <v>11</v>
       </c>
       <c r="I54" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="55" ht="22.5" customHeight="1">
@@ -9707,10 +9708,10 @@
         <v>7006.0</v>
       </c>
       <c r="B55" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C55" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D55" s="12">
         <v>46021.0</v>
@@ -9728,7 +9729,7 @@
         <v>11</v>
       </c>
       <c r="I55" s="11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="56" ht="22.5" customHeight="1">
@@ -9736,33 +9737,39 @@
         <v>7007.0</v>
       </c>
       <c r="B56" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C56" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D56" s="12">
         <v>46023.0</v>
       </c>
-      <c r="E56" s="12"/>
+      <c r="E56" s="12">
+        <v>46023.0</v>
+      </c>
       <c r="F56" s="12">
-        <v>46023.0</v>
-      </c>
-      <c r="G56" s="12"/>
+        <v>46027.0</v>
+      </c>
+      <c r="G56" s="12">
+        <v>46027.0</v>
+      </c>
       <c r="H56" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="I56" s="11"/>
+        <v>11</v>
+      </c>
+      <c r="I56" s="11" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="57" ht="22.5" customHeight="1">
       <c r="A57" s="10">
         <v>7008.0</v>
       </c>
       <c r="B57" s="11" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C57" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D57" s="12">
         <v>46024.0</v>
@@ -9780,7 +9787,7 @@
         <v>11</v>
       </c>
       <c r="I57" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="58" ht="22.5" customHeight="1">
@@ -9788,23 +9795,29 @@
         <v>7009.0</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C58" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D58" s="12">
-        <v>46025.0</v>
-      </c>
-      <c r="E58" s="12"/>
+        <v>46027.0</v>
+      </c>
+      <c r="E58" s="12">
+        <v>46027.0</v>
+      </c>
       <c r="F58" s="12">
-        <v>46026.0</v>
-      </c>
-      <c r="G58" s="12"/>
+        <v>46028.0</v>
+      </c>
+      <c r="G58" s="12">
+        <v>46027.0</v>
+      </c>
       <c r="H58" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="I58" s="11"/>
+        <v>11</v>
+      </c>
+      <c r="I58" s="11" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="5"/>
@@ -16455,50 +16468,50 @@
   <sheetData>
     <row r="1" ht="22.5" customHeight="1">
       <c r="A1" s="26" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" ht="22.5" customHeight="1">
       <c r="A2" s="6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" ht="22.5" customHeight="1">
       <c r="A3" s="6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" ht="22.5" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" ht="22.5" customHeight="1">
       <c r="A5" s="6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" ht="22.5" customHeight="1">
       <c r="A6" s="6" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>